<commit_message>
avances diseño gráfico, consulta de mascota, actualizar domicilio, modificación paso 4 de registro de mascota perdida
</commit_message>
<xml_diff>
--- a/Producto Salud Mascotas/003-Definición del sistema de información/trash.diseño_grafico_checklist.xlsx
+++ b/Producto Salud Mascotas/003-Definición del sistema de información/trash.diseño_grafico_checklist.xlsx
@@ -9,8 +9,6 @@
   <sheets>
     <sheet name="frontend" sheetId="1" r:id="rId1"/>
     <sheet name="backend" sheetId="4" r:id="rId2"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -1728,10 +1726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1823,7 +1821,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75">
+    <row r="17" spans="1:2" ht="15.75">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -1831,7 +1829,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="6" customFormat="1" ht="15.75">
+    <row r="18" spans="1:2" s="6" customFormat="1" ht="15.75">
       <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
@@ -1839,52 +1837,39 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75">
+    <row r="19" spans="1:2" ht="15.75">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:7" ht="18.75">
+    <row r="20" spans="1:2" ht="18.75">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75">
+    <row r="21" spans="1:2" ht="15.75">
       <c r="A21" s="4"/>
-      <c r="F21">
-        <v>700</v>
-      </c>
-      <c r="G21">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="18.75">
+    </row>
+    <row r="22" spans="1:2" ht="18.75">
       <c r="A22" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F22">
-        <f>G22*F21/G21</f>
-        <v>3500</v>
-      </c>
-      <c r="G22">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.75">
+    </row>
+    <row r="23" spans="1:2" ht="15.75">
       <c r="A23" s="4"/>
     </row>
-    <row r="24" spans="1:7" ht="18.75">
+    <row r="24" spans="1:2" ht="18.75">
       <c r="A24" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75">
+    <row r="25" spans="1:2" ht="15.75">
       <c r="A25" s="4"/>
     </row>
-    <row r="26" spans="1:7" ht="18.75">
+    <row r="26" spans="1:2" ht="18.75">
       <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="6" customFormat="1" ht="15.75">
+    <row r="27" spans="1:2" s="6" customFormat="1" ht="15.75">
       <c r="A27" s="5" t="s">
         <v>24</v>
       </c>
@@ -1892,7 +1877,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="6" customFormat="1" ht="15.75">
+    <row r="28" spans="1:2" s="6" customFormat="1" ht="15.75">
       <c r="A28" s="5" t="s">
         <v>25</v>
       </c>
@@ -1900,7 +1885,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="6" customFormat="1" ht="15.75">
+    <row r="29" spans="1:2" s="6" customFormat="1" ht="15.75">
       <c r="A29" s="5" t="s">
         <v>26</v>
       </c>
@@ -1908,7 +1893,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="6" customFormat="1" ht="15.75">
+    <row r="30" spans="1:2" s="6" customFormat="1" ht="15.75">
       <c r="A30" s="5" t="s">
         <v>27</v>
       </c>
@@ -1916,7 +1901,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="6" customFormat="1" ht="15.75">
+    <row r="31" spans="1:2" s="6" customFormat="1" ht="15.75">
       <c r="A31" s="5" t="s">
         <v>28</v>
       </c>
@@ -1924,7 +1909,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="6" customFormat="1" ht="15.75">
+    <row r="32" spans="1:2" s="6" customFormat="1" ht="15.75">
       <c r="A32" s="5" t="s">
         <v>29</v>
       </c>
@@ -2215,30 +2200,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
avances diseño gráfico, nueva pantalla registrar encontrada. Otros cambios menores (ver log_cambios.txt)
</commit_message>
<xml_diff>
--- a/Producto Salud Mascotas/003-Definición del sistema de información/trash.diseño_grafico_checklist.xlsx
+++ b/Producto Salud Mascotas/003-Definición del sistema de información/trash.diseño_grafico_checklist.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
   <si>
     <r>
       <t>·</t>
@@ -1728,8 +1728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21:I25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1759,10 +1759,16 @@
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="5" spans="1:2" ht="15.75">
       <c r="A5" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75">
@@ -1959,8 +1965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Avances diseño gráfico. creo registro y consulta de mascota. otras modificaciones.
</commit_message>
<xml_diff>
--- a/Producto Salud Mascotas/003-Definición del sistema de información/trash.diseño_grafico_checklist.xlsx
+++ b/Producto Salud Mascotas/003-Definición del sistema de información/trash.diseño_grafico_checklist.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="56">
   <si>
     <r>
       <t>·</t>
@@ -1729,7 +1729,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1780,6 +1780,9 @@
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="8" spans="1:2" ht="15.75">
       <c r="A8" s="3" t="s">
@@ -1795,10 +1798,16 @@
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="11" spans="1:2" ht="15.75">
       <c r="A11" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18.75">

</xml_diff>

<commit_message>
avances diseño gráfico, notificación de reencuentro no confirmado y listado de mascotas perdidas.
</commit_message>
<xml_diff>
--- a/Producto Salud Mascotas/003-Definición del sistema de información/trash.diseño_grafico_checklist.xlsx
+++ b/Producto Salud Mascotas/003-Definición del sistema de información/trash.diseño_grafico_checklist.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
   <si>
     <r>
       <t>·</t>
@@ -1729,7 +1729,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1792,6 +1792,9 @@
     <row r="9" spans="1:2" ht="15.75">
       <c r="A9" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75">

</xml_diff>

<commit_message>
avances diseño, listado de mascotas encontradas, reclamo de mascota.
</commit_message>
<xml_diff>
--- a/Producto Salud Mascotas/003-Definición del sistema de información/trash.diseño_grafico_checklist.xlsx
+++ b/Producto Salud Mascotas/003-Definición del sistema de información/trash.diseño_grafico_checklist.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="56">
   <si>
     <r>
       <t>·</t>
@@ -1729,7 +1729,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1787,6 +1787,9 @@
     <row r="8" spans="1:2" ht="15.75">
       <c r="A8" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75">

</xml_diff>